<commit_message>
Vorarbeit Ausarbeitung und Update  Messwerte.xlsx
</commit_message>
<xml_diff>
--- a/Versuch-2-2_Stehende_Wellen_und_Beugung/Versuchsdaten/Messwerte.xlsx
+++ b/Versuch-2-2_Stehende_Wellen_und_Beugung/Versuchsdaten/Messwerte.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benny\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BBB804-6C9F-48E2-8203-13114750914A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69214D2B-300E-424A-B20B-9AF2D0622839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{DB98A966-C5DC-49F7-87CC-797EEE1E23DC}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="20">
   <si>
     <t>Intensität in V</t>
   </si>
@@ -97,11 +97,21 @@
     </r>
   </si>
   <si>
+    <t>Messunsicherheit Uᵤ</t>
+  </si>
+  <si>
+    <t>θ in °</t>
+  </si>
+  <si>
+    <t>U_θ in °</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Winkel </t>
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -116,15 +126,17 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">₂ in </t>
+      <t xml:space="preserve">₁ in </t>
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -140,15 +152,17 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">₃ in </t>
+      <t xml:space="preserve">₂ in </t>
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -164,15 +178,17 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">₁ in </t>
+      <t xml:space="preserve">₃ in </t>
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -183,14 +199,12 @@
     </r>
   </si>
   <si>
-    <t>Messunsicherheit Uᵤ</t>
-  </si>
-  <si>
     <r>
       <t>Mittelwert U</t>
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -200,6 +214,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -214,7 +229,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,6 +241,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -243,7 +276,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -630,11 +663,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -654,28 +724,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
@@ -713,18 +768,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -773,6 +816,60 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4406,8 +4503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8ABD8C-5FED-4053-85DB-106CAF30C057}">
   <dimension ref="B1:P45"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V25" sqref="V25"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4428,13 +4525,13 @@
   <sheetData>
     <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="32"/>
+      <c r="D2" s="23"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="6">
@@ -4443,7 +4540,7 @@
       <c r="C3" s="5">
         <v>0.16969999999999999</v>
       </c>
-      <c r="D3" s="33"/>
+      <c r="D3" s="24"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
@@ -4452,7 +4549,7 @@
       <c r="C4" s="3">
         <v>1.9653</v>
       </c>
-      <c r="D4" s="33"/>
+      <c r="D4" s="24"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
@@ -4461,7 +4558,7 @@
       <c r="C5" s="3">
         <v>4.9169999999999998</v>
       </c>
-      <c r="D5" s="33"/>
+      <c r="D5" s="24"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
@@ -4470,7 +4567,7 @@
       <c r="C6" s="3">
         <v>7.3167999999999997</v>
       </c>
-      <c r="D6" s="33"/>
+      <c r="D6" s="24"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="4">
@@ -4479,7 +4576,7 @@
       <c r="C7" s="3">
         <v>8.0343999999999998</v>
       </c>
-      <c r="D7" s="33"/>
+      <c r="D7" s="24"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
@@ -4488,7 +4585,7 @@
       <c r="C8" s="3">
         <v>7.6345000000000001</v>
       </c>
-      <c r="D8" s="33"/>
+      <c r="D8" s="24"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
@@ -4497,7 +4594,7 @@
       <c r="C9" s="3">
         <v>5.7352999999999996</v>
       </c>
-      <c r="D9" s="33"/>
+      <c r="D9" s="24"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
@@ -4506,7 +4603,7 @@
       <c r="C10" s="3">
         <v>1.4112</v>
       </c>
-      <c r="D10" s="33"/>
+      <c r="D10" s="24"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="4">
@@ -4515,7 +4612,7 @@
       <c r="C11" s="3">
         <v>0.17926</v>
       </c>
-      <c r="D11" s="33"/>
+      <c r="D11" s="24"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
@@ -4524,7 +4621,7 @@
       <c r="C12" s="3">
         <v>1.1798</v>
       </c>
-      <c r="D12" s="33"/>
+      <c r="D12" s="24"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
@@ -4533,7 +4630,7 @@
       <c r="C13" s="3">
         <v>4.6470000000000002</v>
       </c>
-      <c r="D13" s="33"/>
+      <c r="D13" s="24"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
@@ -4542,7 +4639,7 @@
       <c r="C14" s="3">
         <v>7.4325999999999999</v>
       </c>
-      <c r="D14" s="33"/>
+      <c r="D14" s="24"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
@@ -4551,7 +4648,7 @@
       <c r="C15" s="3">
         <v>8.532</v>
       </c>
-      <c r="D15" s="33"/>
+      <c r="D15" s="24"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="4">
@@ -4560,7 +4657,7 @@
       <c r="C16" s="3">
         <v>8.4461999999999993</v>
       </c>
-      <c r="D16" s="33"/>
+      <c r="D16" s="24"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="4">
@@ -4569,7 +4666,7 @@
       <c r="C17" s="3">
         <v>6.3071999999999999</v>
       </c>
-      <c r="D17" s="33"/>
+      <c r="D17" s="24"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="4">
@@ -4578,7 +4675,7 @@
       <c r="C18" s="3">
         <v>3.0878000000000001</v>
       </c>
-      <c r="D18" s="33"/>
+      <c r="D18" s="24"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="4">
@@ -4587,7 +4684,7 @@
       <c r="C19" s="3">
         <v>0.53117999999999999</v>
       </c>
-      <c r="D19" s="33"/>
+      <c r="D19" s="24"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="4">
@@ -4596,7 +4693,7 @@
       <c r="C20" s="3">
         <v>1.7968</v>
       </c>
-      <c r="D20" s="33"/>
+      <c r="D20" s="24"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="4">
@@ -4605,7 +4702,7 @@
       <c r="C21" s="3">
         <v>4.4162999999999997</v>
       </c>
-      <c r="D21" s="33"/>
+      <c r="D21" s="24"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="4">
@@ -4614,7 +4711,7 @@
       <c r="C22" s="3">
         <v>7.1951000000000001</v>
       </c>
-      <c r="D22" s="33"/>
+      <c r="D22" s="24"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="4">
@@ -4623,7 +4720,7 @@
       <c r="C23" s="3">
         <v>8.5310000000000006</v>
       </c>
-      <c r="D23" s="33"/>
+      <c r="D23" s="24"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="4">
@@ -4632,7 +4729,7 @@
       <c r="C24" s="3">
         <v>9.0498999999999992</v>
       </c>
-      <c r="D24" s="33"/>
+      <c r="D24" s="24"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="4">
@@ -4641,7 +4738,7 @@
       <c r="C25" s="3">
         <v>7.5515999999999996</v>
       </c>
-      <c r="D25" s="33"/>
+      <c r="D25" s="24"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="4">
@@ -4650,7 +4747,7 @@
       <c r="C26" s="3">
         <v>4.2053000000000003</v>
       </c>
-      <c r="D26" s="33"/>
+      <c r="D26" s="24"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="4">
@@ -4659,7 +4756,7 @@
       <c r="C27" s="3">
         <v>1.7835000000000001</v>
       </c>
-      <c r="D27" s="33"/>
+      <c r="D27" s="24"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="4">
@@ -4668,7 +4765,7 @@
       <c r="C28" s="3">
         <v>1.4283999999999999</v>
       </c>
-      <c r="D28" s="33"/>
+      <c r="D28" s="24"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="4">
@@ -4677,7 +4774,7 @@
       <c r="C29" s="3">
         <v>4.1848999999999998</v>
       </c>
-      <c r="D29" s="33"/>
+      <c r="D29" s="24"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="4">
@@ -4686,7 +4783,7 @@
       <c r="C30" s="3">
         <v>6.0621999999999998</v>
       </c>
-      <c r="D30" s="33"/>
+      <c r="D30" s="24"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="4">
@@ -4695,7 +4792,7 @@
       <c r="C31" s="3">
         <v>8.6432000000000002</v>
       </c>
-      <c r="D31" s="33"/>
+      <c r="D31" s="24"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="4">
@@ -4704,7 +4801,7 @@
       <c r="C32" s="3">
         <v>8.9794</v>
       </c>
-      <c r="D32" s="33"/>
+      <c r="D32" s="24"/>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B33" s="4">
@@ -4713,7 +4810,7 @@
       <c r="C33" s="3">
         <v>7.8536000000000001</v>
       </c>
-      <c r="D33" s="33"/>
+      <c r="D33" s="24"/>
     </row>
     <row r="34" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="2">
@@ -4722,83 +4819,83 @@
       <c r="C34" s="1">
         <v>5.8124000000000002</v>
       </c>
-      <c r="D34" s="33"/>
+      <c r="D34" s="24"/>
     </row>
     <row r="37" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="2:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="12" t="s">
+      <c r="B38" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="D38" s="41" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B39" s="15">
+      <c r="B39" s="10">
         <v>58</v>
       </c>
-      <c r="C39" s="16" t="s">
+      <c r="C39" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D39" s="17"/>
-      <c r="F39" s="23" t="s">
+      <c r="D39" s="12"/>
+      <c r="F39" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="G39" s="8">
+      <c r="G39" s="7">
         <f>AVERAGE(D40:D45)</f>
         <v>32.666666666666664</v>
       </c>
-      <c r="H39" s="9" t="s">
+      <c r="H39" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I39" s="8">
+      <c r="I39" s="7">
         <f>_xlfn.STDEV.S(D40:D45)/SQRT(COUNT(D40:D45))*2</f>
         <v>2.4585451886114371</v>
       </c>
-      <c r="J39" s="24" t="s">
+      <c r="J39" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="L39" s="23" t="s">
+      <c r="L39" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="M39" s="9">
+      <c r="M39" s="8">
         <f>2*PI()/G42</f>
         <v>0.19214633966910047</v>
       </c>
-      <c r="N39" s="9" t="s">
+      <c r="N39" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="O39" s="8">
+      <c r="O39" s="7">
         <f>ABS(-2*PI()/(G42)^2)*I42</f>
         <v>1.4690087130665172E-2</v>
       </c>
-      <c r="P39" s="24" t="s">
+      <c r="P39" s="19" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B40" s="18">
+      <c r="B40" s="13">
         <v>66</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D40" s="19">
+      <c r="D40" s="14">
         <f>(B40-B39)*4</f>
         <v>32</v>
       </c>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B41" s="18">
+      <c r="B41" s="13">
         <v>75</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D41" s="19">
+      <c r="D41" s="14">
         <f t="shared" ref="D41:D45" si="0">(B41-B40)*4</f>
         <v>36</v>
       </c>
@@ -4807,83 +4904,83 @@
       </c>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B42" s="18">
+      <c r="B42" s="13">
         <v>82</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D42" s="19">
+      <c r="D42" s="14">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="F42" s="23" t="s">
+      <c r="F42" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="G42" s="25">
+      <c r="G42" s="20">
         <f>ROUND(G39,1-INT(LOG(ABS(I39))))</f>
         <v>32.700000000000003</v>
       </c>
-      <c r="H42" s="9" t="s">
+      <c r="H42" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I42" s="25">
+      <c r="I42" s="20">
         <f>ROUNDUP(I39,1-INT(LOG(ABS(I39))))</f>
         <v>2.5</v>
       </c>
-      <c r="J42" s="24" t="s">
+      <c r="J42" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="L42" s="23" t="s">
+      <c r="L42" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="M42" s="26">
+      <c r="M42" s="21">
         <f>ROUND(M39,1-INT(LOG(ABS(O39))))</f>
         <v>0.192</v>
       </c>
-      <c r="N42" s="9" t="s">
+      <c r="N42" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="O42" s="25">
+      <c r="O42" s="20">
         <f>ROUNDUP(O39,1-INT(LOG(ABS(O39))))</f>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="P42" s="24" t="s">
+      <c r="P42" s="19" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B43" s="18">
+      <c r="B43" s="13">
         <v>91</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D43" s="19">
+      <c r="D43" s="14">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B44" s="18">
+      <c r="B44" s="13">
         <v>99</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D44" s="19">
+      <c r="D44" s="14">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
     </row>
     <row r="45" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="20">
+      <c r="B45" s="15">
         <v>107</v>
       </c>
-      <c r="C45" s="21" t="s">
+      <c r="C45" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D45" s="22">
+      <c r="D45" s="17">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
@@ -4896,10 +4993,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B1AE1D-67A1-4331-B488-767FEB15DA6A}">
-  <dimension ref="B1:I37"/>
+  <dimension ref="B1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="M48" sqref="M48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4910,681 +5007,828 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I1" s="31"/>
+      <c r="I1" s="22"/>
     </row>
     <row r="2" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="32"/>
+      <c r="I2" s="23"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="36">
+      <c r="B3" s="27">
         <v>-60</v>
       </c>
-      <c r="C3" s="39">
+      <c r="C3" s="30">
         <v>0.21092</v>
       </c>
-      <c r="D3" s="40">
+      <c r="D3" s="31">
         <v>0.19389000000000001</v>
       </c>
-      <c r="E3" s="41">
+      <c r="E3" s="32">
         <v>0.15306</v>
       </c>
-      <c r="F3" s="34">
+      <c r="F3" s="25">
         <f>ROUND(AVERAGE(C3:E3),1-INT(LOG(ABS(_xlfn.STDEV.S(C3:E3)/SQRT(COUNT(C3:E3))*2))))</f>
         <v>0.186</v>
       </c>
-      <c r="G3" s="35">
+      <c r="G3" s="26">
         <f>ROUNDUP(_xlfn.STDEV.S(C3:E3)/SQRT(COUNT(C3:E3))*2,1-INT(LOG(ABS(_xlfn.STDEV.S(C3:E3)/SQRT(COUNT(C3:E3))*2))))</f>
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="I3" s="33"/>
+      <c r="I3" s="24"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
         <v>-55</v>
       </c>
-      <c r="C4" s="42">
+      <c r="C4" s="33">
         <v>0.11987</v>
       </c>
-      <c r="D4" s="43">
+      <c r="D4" s="34">
         <v>0.26127</v>
       </c>
-      <c r="E4" s="44">
+      <c r="E4" s="35">
         <v>0.13519</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="13">
         <f t="shared" ref="F4:F27" si="0">ROUND(AVERAGE(C4:E4),1-INT(LOG(ABS(_xlfn.STDEV.S(C4:E4)/SQRT(COUNT(C4:E4))*2))))</f>
         <v>0.17199999999999999</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="14">
         <f t="shared" ref="G4:G27" si="1">ROUNDUP(_xlfn.STDEV.S(C4:E4)/SQRT(COUNT(C4:E4))*2,1-INT(LOG(ABS(_xlfn.STDEV.S(C4:E4)/SQRT(COUNT(C4:E4))*2))))</f>
         <v>0.09</v>
       </c>
-      <c r="I4" s="33"/>
+      <c r="I4" s="24"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="36">
+      <c r="B5" s="27">
         <v>-50</v>
       </c>
-      <c r="C5" s="42">
+      <c r="C5" s="33">
         <v>0.97433999999999998</v>
       </c>
-      <c r="D5" s="43">
+      <c r="D5" s="34">
         <v>1.0980799999999999</v>
       </c>
-      <c r="E5" s="44">
+      <c r="E5" s="35">
         <v>1.15873</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="13">
         <f t="shared" si="0"/>
         <v>1.08</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="14">
         <f t="shared" si="1"/>
         <v>0.11</v>
       </c>
-      <c r="I5" s="33"/>
+      <c r="I5" s="24"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>-45</v>
       </c>
-      <c r="C6" s="42">
+      <c r="C6" s="33">
         <v>1.7385999999999999</v>
       </c>
-      <c r="D6" s="43">
+      <c r="D6" s="34">
         <v>1.62026</v>
       </c>
-      <c r="E6" s="44">
+      <c r="E6" s="35">
         <v>1.79813</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="13">
         <f t="shared" si="0"/>
         <v>1.72</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="14">
         <f t="shared" si="1"/>
         <v>0.11</v>
       </c>
-      <c r="I6" s="33"/>
+      <c r="I6" s="24"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="36">
+      <c r="B7" s="27">
         <v>-40</v>
       </c>
-      <c r="C7" s="42">
+      <c r="C7" s="33">
         <v>2.2366000000000001</v>
       </c>
-      <c r="D7" s="43">
+      <c r="D7" s="34">
         <v>2.1591200000000002</v>
       </c>
-      <c r="E7" s="44">
+      <c r="E7" s="35">
         <v>2.0592800000000002</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="13">
         <f t="shared" si="0"/>
         <v>2.15</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="14">
         <f t="shared" si="1"/>
         <v>0.11</v>
       </c>
-      <c r="I7" s="33"/>
+      <c r="I7" s="24"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>-35</v>
       </c>
-      <c r="C8" s="42">
+      <c r="C8" s="33">
         <v>1.3924000000000001</v>
       </c>
-      <c r="D8" s="43">
+      <c r="D8" s="34">
         <v>1.3045899999999999</v>
       </c>
-      <c r="E8" s="44">
+      <c r="E8" s="35">
         <v>1.4672799999999999</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="13">
         <f t="shared" si="0"/>
         <v>1.3879999999999999</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="14">
         <f t="shared" si="1"/>
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="I8" s="33"/>
+      <c r="I8" s="24"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="36">
+      <c r="B9" s="27">
         <v>-30</v>
       </c>
-      <c r="C9" s="42">
+      <c r="C9" s="33">
         <v>0.25861000000000001</v>
       </c>
-      <c r="D9" s="43">
+      <c r="D9" s="34">
         <v>0.410026</v>
       </c>
-      <c r="E9" s="44">
+      <c r="E9" s="35">
         <v>0.29674</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="13">
         <f t="shared" si="0"/>
         <v>0.32200000000000001</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="14">
         <f t="shared" si="1"/>
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="I9" s="33"/>
+      <c r="I9" s="24"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
         <v>-25</v>
       </c>
-      <c r="C10" s="42">
+      <c r="C10" s="33">
         <v>2.5242</v>
       </c>
-      <c r="D10" s="43">
+      <c r="D10" s="34">
         <v>2.59579</v>
       </c>
-      <c r="E10" s="44">
+      <c r="E10" s="35">
         <v>2.54115</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="13">
         <f t="shared" si="0"/>
         <v>2.5539999999999998</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="14">
         <f t="shared" si="1"/>
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="I10" s="33"/>
+      <c r="I10" s="24"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="36">
+      <c r="B11" s="27">
         <v>-20</v>
       </c>
-      <c r="C11" s="42">
+      <c r="C11" s="33">
         <v>6.0397999999999996</v>
       </c>
-      <c r="D11" s="43">
+      <c r="D11" s="34">
         <v>6.1743300000000003</v>
       </c>
-      <c r="E11" s="44">
+      <c r="E11" s="35">
         <v>6.2361500000000003</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="13">
         <f t="shared" si="0"/>
         <v>6.15</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="14">
         <f t="shared" si="1"/>
         <v>0.12</v>
       </c>
-      <c r="I11" s="33"/>
+      <c r="I11" s="24"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
         <v>-15</v>
       </c>
-      <c r="C12" s="42">
+      <c r="C12" s="33">
         <v>6.5486000000000004</v>
       </c>
-      <c r="D12" s="43">
+      <c r="D12" s="34">
         <v>6.7005800000000004</v>
       </c>
-      <c r="E12" s="44">
+      <c r="E12" s="35">
         <v>6.5704000000000002</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="13">
         <f t="shared" si="0"/>
         <v>6.6070000000000002</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="14">
         <f t="shared" si="1"/>
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="I12" s="33"/>
+      <c r="I12" s="24"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="36">
+      <c r="B13" s="27">
         <v>-10</v>
       </c>
-      <c r="C13" s="42">
+      <c r="C13" s="33">
         <v>3.2199999999999999E-2</v>
       </c>
-      <c r="D13" s="43">
+      <c r="D13" s="34">
         <v>2.5229999999999999E-2</v>
       </c>
-      <c r="E13" s="44">
+      <c r="E13" s="35">
         <v>0.17621000000000001</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="13">
         <f t="shared" si="0"/>
         <v>7.8E-2</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="14">
         <f t="shared" si="1"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="I13" s="33"/>
+      <c r="I13" s="24"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
         <v>-5</v>
       </c>
-      <c r="C14" s="42">
+      <c r="C14" s="33">
         <v>4.2487000000000004</v>
       </c>
-      <c r="D14" s="43">
+      <c r="D14" s="34">
         <v>4.1212299999999997</v>
       </c>
-      <c r="E14" s="44">
+      <c r="E14" s="35">
         <v>4.09701</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F14" s="13">
         <f t="shared" si="0"/>
         <v>4.1559999999999997</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G14" s="14">
         <f t="shared" si="1"/>
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="I14" s="33"/>
+      <c r="I14" s="24"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="36">
+      <c r="B15" s="27">
         <v>0</v>
       </c>
-      <c r="C15" s="42">
+      <c r="C15" s="33">
         <v>8.3575999999999997</v>
       </c>
-      <c r="D15" s="43">
+      <c r="D15" s="34">
         <v>8.4229800000000008</v>
       </c>
-      <c r="E15" s="44">
+      <c r="E15" s="35">
         <v>8.3818199999999994</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F15" s="13">
         <f t="shared" si="0"/>
         <v>8.3870000000000005</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="14">
         <f t="shared" si="1"/>
         <v>3.9E-2</v>
       </c>
-      <c r="I15" s="33"/>
+      <c r="I15" s="24"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="4">
         <v>5</v>
       </c>
-      <c r="C16" s="42">
+      <c r="C16" s="33">
         <v>4.3907999999999996</v>
       </c>
-      <c r="D16" s="43">
+      <c r="D16" s="34">
         <v>4.56691</v>
       </c>
-      <c r="E16" s="44">
+      <c r="E16" s="35">
         <v>4.3925799999999997</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="13">
         <f t="shared" si="0"/>
         <v>4.45</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="14">
         <f t="shared" si="1"/>
         <v>0.12</v>
       </c>
-      <c r="I16" s="33"/>
+      <c r="I16" s="24"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="36">
+      <c r="B17" s="27">
         <v>10</v>
       </c>
-      <c r="C17" s="42">
+      <c r="C17" s="33">
         <v>0.55335000000000001</v>
       </c>
-      <c r="D17" s="43">
+      <c r="D17" s="34">
         <v>0.65671000000000002</v>
       </c>
-      <c r="E17" s="44">
+      <c r="E17" s="35">
         <v>0.53881999999999997</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F17" s="13">
         <f t="shared" si="0"/>
         <v>0.58299999999999996</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="14">
         <f t="shared" si="1"/>
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="I17" s="33"/>
+      <c r="I17" s="24"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="4">
         <v>15</v>
       </c>
-      <c r="C18" s="42">
+      <c r="C18" s="33">
         <v>6.0747999999999998</v>
       </c>
-      <c r="D18" s="43">
+      <c r="D18" s="34">
         <v>6.2208199999999998</v>
       </c>
-      <c r="E18" s="44">
+      <c r="E18" s="35">
         <v>6.2777500000000002</v>
       </c>
-      <c r="F18" s="18">
+      <c r="F18" s="13">
         <f t="shared" si="0"/>
         <v>6.19</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="14">
         <f t="shared" si="1"/>
         <v>0.13</v>
       </c>
-      <c r="I18" s="33"/>
+      <c r="I18" s="24"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="36">
+      <c r="B19" s="27">
         <v>20</v>
       </c>
-      <c r="C19" s="42">
+      <c r="C19" s="33">
         <v>7.3945999999999996</v>
       </c>
-      <c r="D19" s="43">
+      <c r="D19" s="34">
         <v>7.2396900000000004</v>
       </c>
-      <c r="E19" s="44">
+      <c r="E19" s="35">
         <v>7.2876000000000003</v>
       </c>
-      <c r="F19" s="18">
+      <c r="F19" s="13">
         <f t="shared" si="0"/>
         <v>7.3070000000000004</v>
       </c>
-      <c r="G19" s="19">
+      <c r="G19" s="14">
         <f t="shared" si="1"/>
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="I19" s="33"/>
+      <c r="I19" s="24"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="4">
         <v>25</v>
       </c>
-      <c r="C20" s="42">
+      <c r="C20" s="33">
         <v>3.5390000000000001</v>
       </c>
-      <c r="D20" s="43">
+      <c r="D20" s="34">
         <v>3.36077</v>
       </c>
-      <c r="E20" s="44">
+      <c r="E20" s="35">
         <v>3.2124100000000002</v>
       </c>
-      <c r="F20" s="18">
+      <c r="F20" s="13">
         <f t="shared" si="0"/>
         <v>3.37</v>
       </c>
-      <c r="G20" s="19">
+      <c r="G20" s="14">
         <f t="shared" si="1"/>
         <v>0.19</v>
       </c>
-      <c r="I20" s="33"/>
+      <c r="I20" s="24"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="36">
+      <c r="B21" s="27">
         <v>30</v>
       </c>
-      <c r="C21" s="42">
+      <c r="C21" s="33">
         <v>0.28608</v>
       </c>
-      <c r="D21" s="43">
+      <c r="D21" s="34">
         <v>0.32274999999999998</v>
       </c>
-      <c r="E21" s="44">
+      <c r="E21" s="35">
         <v>0.30667</v>
       </c>
-      <c r="F21" s="18">
+      <c r="F21" s="13">
         <f t="shared" si="0"/>
         <v>0.30499999999999999</v>
       </c>
-      <c r="G21" s="19">
+      <c r="G21" s="14">
         <f t="shared" si="1"/>
         <v>2.2000000000000002E-2</v>
       </c>
-      <c r="I21" s="33"/>
+      <c r="I21" s="24"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="4">
         <v>35</v>
       </c>
-      <c r="C22" s="42">
+      <c r="C22" s="33">
         <v>1.4377</v>
       </c>
-      <c r="D22" s="43">
+      <c r="D22" s="34">
         <v>1.5612600000000001</v>
       </c>
-      <c r="E22" s="44">
+      <c r="E22" s="35">
         <v>1.7411099999999999</v>
       </c>
-      <c r="F22" s="18">
+      <c r="F22" s="13">
         <f t="shared" si="0"/>
         <v>1.58</v>
       </c>
-      <c r="G22" s="19">
+      <c r="G22" s="14">
         <f t="shared" si="1"/>
         <v>0.18000000000000002</v>
       </c>
-      <c r="I22" s="33"/>
+      <c r="I22" s="24"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="36">
+      <c r="B23" s="27">
         <v>40</v>
       </c>
-      <c r="C23" s="42">
+      <c r="C23" s="33">
         <v>3.0691000000000002</v>
       </c>
-      <c r="D23" s="43">
+      <c r="D23" s="34">
         <v>3.01681</v>
       </c>
-      <c r="E23" s="44">
+      <c r="E23" s="35">
         <v>3.05532</v>
       </c>
-      <c r="F23" s="18">
+      <c r="F23" s="13">
         <f t="shared" si="0"/>
         <v>3.0470000000000002</v>
       </c>
-      <c r="G23" s="19">
+      <c r="G23" s="14">
         <f t="shared" si="1"/>
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="I23" s="33"/>
+      <c r="I23" s="24"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="4">
         <v>45</v>
       </c>
-      <c r="C24" s="42">
+      <c r="C24" s="33">
         <v>2.3662000000000001</v>
       </c>
-      <c r="D24" s="43">
+      <c r="D24" s="34">
         <v>2.2650600000000001</v>
       </c>
-      <c r="E24" s="44">
+      <c r="E24" s="35">
         <v>2.1782599999999999</v>
       </c>
-      <c r="F24" s="18">
+      <c r="F24" s="13">
         <f t="shared" si="0"/>
         <v>2.27</v>
       </c>
-      <c r="G24" s="19">
+      <c r="G24" s="14">
         <f t="shared" si="1"/>
         <v>0.11</v>
       </c>
-      <c r="I24" s="33"/>
+      <c r="I24" s="24"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="36">
+      <c r="B25" s="27">
         <v>50</v>
       </c>
-      <c r="C25" s="42">
+      <c r="C25" s="33">
         <v>1.5174000000000001</v>
       </c>
-      <c r="D25" s="43">
+      <c r="D25" s="34">
         <v>1.6735899999999999</v>
       </c>
-      <c r="E25" s="44">
+      <c r="E25" s="35">
         <v>1.7435499999999999</v>
       </c>
-      <c r="F25" s="18">
+      <c r="F25" s="13">
         <f t="shared" si="0"/>
         <v>1.64</v>
       </c>
-      <c r="G25" s="19">
+      <c r="G25" s="14">
         <f t="shared" si="1"/>
         <v>0.14000000000000001</v>
       </c>
-      <c r="I25" s="33"/>
+      <c r="I25" s="24"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="4">
         <v>55</v>
       </c>
-      <c r="C26" s="42">
+      <c r="C26" s="33">
         <v>0.78920999999999997</v>
       </c>
-      <c r="D26" s="43">
+      <c r="D26" s="34">
         <v>0.77537</v>
       </c>
-      <c r="E26" s="44">
+      <c r="E26" s="35">
         <v>0.73163999999999996</v>
       </c>
-      <c r="F26" s="18">
+      <c r="F26" s="13">
         <f t="shared" si="0"/>
         <v>0.76500000000000001</v>
       </c>
-      <c r="G26" s="19">
+      <c r="G26" s="14">
         <f t="shared" si="1"/>
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="I26" s="33"/>
+      <c r="I26" s="24"/>
     </row>
     <row r="27" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="38">
+      <c r="B27" s="29">
         <v>60</v>
       </c>
-      <c r="C27" s="45">
+      <c r="C27" s="36">
         <v>0.20322000000000001</v>
       </c>
-      <c r="D27" s="46">
+      <c r="D27" s="37">
         <v>0.33983000000000002</v>
       </c>
-      <c r="E27" s="47">
+      <c r="E27" s="38">
         <v>0.34433000000000002</v>
       </c>
-      <c r="F27" s="20">
+      <c r="F27" s="15">
         <f t="shared" si="0"/>
         <v>0.29599999999999999</v>
       </c>
-      <c r="G27" s="22">
+      <c r="G27" s="17">
         <f t="shared" si="1"/>
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="I27" s="33"/>
+      <c r="I27" s="24"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="33"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
-      <c r="I28" s="33"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="I28" s="24"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="33"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
-      <c r="I29" s="33"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+      <c r="I29" s="24"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="33"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="I30" s="33"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="I30" s="24"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="33"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
-      <c r="I31" s="33"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="I31" s="24"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="33"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="33"/>
-      <c r="I32" s="33"/>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="33"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="37"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="33"/>
-      <c r="I33" s="33"/>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="33"/>
-      <c r="C34" s="37"/>
-      <c r="D34" s="37"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="33"/>
-      <c r="I34" s="33"/>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I35" s="31"/>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I36" s="31"/>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I37" s="31"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="I32" s="24"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="24"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="I33" s="24"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B34" s="24"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="I34" s="24"/>
+    </row>
+    <row r="35" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I35" s="22"/>
+    </row>
+    <row r="36" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I36" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="J36" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="K36" s="49" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I37" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="J37" s="55">
+        <f>ROUND(ASIN(((-3+0.5)*0.0327)/0.09)*180/PI(),0)</f>
+        <v>-65</v>
+      </c>
+      <c r="K37" s="52">
+        <f>ROUNDUP((ABS(SQRT(((-2-1/2)^2)/(90^2-((2*(-2)-1)*32.7/2)^2)))*2.5+ABS(-SQRT(((32.7*(-2)-1/2)^2)/(90^4-((2*(-2)-1)*32.7/2)^2*90^2)))*2)*180/PI(),0)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I38" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J38" s="54">
+        <f>ROUND(ASIN((-2*0.0327)/0.09)*180/PI(),0)</f>
+        <v>-47</v>
+      </c>
+      <c r="K38" s="51">
+        <f>ROUNDUP((ABS(SQRT(((-2)^2)/(90^2-(-2)^2*32.7^2)))*2.5+ABS(-SQRT(((-2)^2*32.7^2)/(90^4-(-2)^2*32.7^2*90^2)))*2)*180/PI(),0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I39" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J39" s="54">
+        <f>ROUND(ASIN(((-2+0.5)*0.0327)/0.09)*180/PI(),1)</f>
+        <v>-33</v>
+      </c>
+      <c r="K39" s="50">
+        <f>ROUNDUP((ABS(SQRT(((-1-1/2)^2)/(90^2-((2*(-1)-1)*32.7/2)^2)))*2.5+ABS(-SQRT(((32.7*(-1)-1/2)^2)/(90^4-((2*(-1)-1)*32.7/2)^2*90^2)))*2)*180/PI(),1)</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I40" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J40" s="3">
+        <f>ROUND(ASIN((-1*0.0327)/0.09)*180/PI(),1)</f>
+        <v>-21.3</v>
+      </c>
+      <c r="K40" s="50">
+        <f>ROUNDUP((ABS(SQRT(((-1)^2)/(90^2-(-1)^2*32.7^2)))*2.5+ABS(-SQRT(((-1)^2*32.7^2)/(90^4-(-1)^2*32.7^2*90^2)))*2)*180/PI(),1)</f>
+        <v>2.3000000000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I41" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J41" s="3">
+        <f>ROUND(ASIN(((-1+0.5)*0.0327)/0.09)*180/PI(),2)</f>
+        <v>-10.47</v>
+      </c>
+      <c r="K41" s="50">
+        <f>ROUNDUP((ABS(SQRT(((0-1/2)^2)/(90^2-((2*(0)-1)*32.7/2)^2)))*2.5+ABS(-SQRT(((32.7*(0)-1/2)^2)/(90^4-((2*(0)-1)*32.7/2)^2*90^2)))*2)*180/PI(),2)</f>
+        <v>0.82000000000000006</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I42" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J42" s="54">
+        <v>0</v>
+      </c>
+      <c r="K42" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I43" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J43" s="3">
+        <f>ROUND(ASIN(((0+0.5)*0.0327)/0.09)*180/PI(),2)</f>
+        <v>10.47</v>
+      </c>
+      <c r="K43" s="50">
+        <f>ROUNDUP((ABS(SQRT(((0-1/2)^2)/(90^2-((2*(0)-1)*32.7/2)^2)))*2.5+ABS(-SQRT(((32.7*(0)-1/2)^2)/(90^4-((2*(0)-1)*32.7/2)^2*90^2)))*2)*180/PI(),2)</f>
+        <v>0.82000000000000006</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I44" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J44" s="3">
+        <f>ROUND(ASIN((1*0.0327)/0.09)*180/PI(),1)</f>
+        <v>21.3</v>
+      </c>
+      <c r="K44" s="50">
+        <f>ROUNDUP((ABS(SQRT(((1)^2)/(90^2-(1)^2*32.7^2)))*2.5+ABS(-SQRT(((1)^2*32.7^2)/(90^4-(1)^2*32.7^2*90^2)))*2)*180/PI(),1)</f>
+        <v>2.3000000000000003</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I45" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J45" s="54">
+        <f>ROUND(ASIN(((1+0.5)*0.0327)/0.09)*180/PI(),1)</f>
+        <v>33</v>
+      </c>
+      <c r="K45" s="50">
+        <f>ROUNDUP((ABS(SQRT(((-1-1/2)^2)/(90^2-((2*(-1)-1)*32.7/2)^2)))*2.5+ABS(-SQRT(((32.7*(-1)-1/2)^2)/(90^4-((2*(-1)-1)*32.7/2)^2*90^2)))*2)*180/PI(),1)</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I46" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J46" s="54">
+        <f>ROUND(ASIN((2*0.0327)/0.09)*180/PI(),0)</f>
+        <v>47</v>
+      </c>
+      <c r="K46" s="51">
+        <f>ROUNDUP((ABS(SQRT(((2)^2)/(90^2-(2)^2*32.7^2)))*2.5+ABS(-SQRT(((2)^2*32.7^2)/(90^4-(2)^2*32.7^2*90^2)))*2)*180/PI(),0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I47" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J47" s="56">
+        <f>ROUND(ASIN(((2+0.5)*0.0327)/0.09)*180/PI(),0)</f>
+        <v>65</v>
+      </c>
+      <c r="K47" s="53">
+        <f>ROUNDUP((ABS(SQRT(((-2-1/2)^2)/(90^2-((2*(-2)-1)*32.7/2)^2)))*2.5+ABS(-SQRT(((32.7*(-2)-1/2)^2)/(90^4-((2*(-2)-1)*32.7/2)^2*90^2)))*2)*180/PI(),0)</f>
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="F3:G27" formulaRange="1"/>
   </ignoredErrors>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>